<commit_message>
Update tests and test data
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/repo/Oz_butterflies_summary.xlsx
+++ b/tests/testthat/testdata/repo/Oz_butterflies_summary.xlsx
@@ -38,18 +38,27 @@
     <t xml:space="preserve">Hesperiidae</t>
   </si>
   <si>
+    <t xml:space="preserve">Notocrypta waigensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suniana sunias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telicota mesoptis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arrhenes dschilus</t>
   </si>
   <si>
-    <t xml:space="preserve">n</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cephrenes augiades</t>
   </si>
   <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hesperilla crypsigramma</t>
   </si>
   <si>
@@ -62,9 +71,6 @@
     <t xml:space="preserve">Netrocoryne repanda</t>
   </si>
   <si>
-    <t xml:space="preserve">Notocrypta waigensis</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ocybadistes ardea</t>
   </si>
   <si>
@@ -98,9 +104,6 @@
     <t xml:space="preserve">Suniana lascivia</t>
   </si>
   <si>
-    <t xml:space="preserve">Suniana sunias</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tagiades japetus</t>
   </si>
   <si>
@@ -119,9 +122,6 @@
     <t xml:space="preserve">Telicota colon</t>
   </si>
   <si>
-    <t xml:space="preserve">Telicota mesoptis</t>
-  </si>
-  <si>
     <t xml:space="preserve">Telicota ohara</t>
   </si>
   <si>
@@ -251,6 +251,9 @@
     <t xml:space="preserve">Nymphalidae</t>
   </si>
   <si>
+    <t xml:space="preserve">Euploea darchia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Acraea andromacha</t>
   </si>
   <si>
@@ -281,9 +284,6 @@
     <t xml:space="preserve">Euploea corinna</t>
   </si>
   <si>
-    <t xml:space="preserve">Euploea darchia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Euploea sylvester</t>
   </si>
   <si>
@@ -365,6 +365,9 @@
     <t xml:space="preserve">Papilionidae</t>
   </si>
   <si>
+    <t xml:space="preserve">Papilio aegeus</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cressida cressida</t>
   </si>
   <si>
@@ -377,9 +380,6 @@
     <t xml:space="preserve">Pachliopta polydorus</t>
   </si>
   <si>
-    <t xml:space="preserve">Papilio aegeus</t>
-  </si>
-  <si>
     <t xml:space="preserve">Papilio ambrax</t>
   </si>
   <si>
@@ -389,6 +389,9 @@
     <t xml:space="preserve">Pieridae</t>
   </si>
   <si>
+    <t xml:space="preserve">Elodina angulipennis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Belenois java</t>
   </si>
   <si>
@@ -407,7 +410,7 @@
     <t xml:space="preserve">Delias nigrina</t>
   </si>
   <si>
-    <t xml:space="preserve">Elodina angulipennis</t>
+    <t xml:space="preserve">Eurema hecabe</t>
   </si>
   <si>
     <t xml:space="preserve">Elodina parthia</t>
@@ -417,9 +420,6 @@
   </si>
   <si>
     <t xml:space="preserve">Eurema brigitta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eurema hecabe</t>
   </si>
   <si>
     <t xml:space="preserve">Eurema laeta</t>
@@ -790,14 +790,10 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="n">
-        <v>47</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2" t="n">
         <v>5</v>
-      </c>
-      <c r="E2" t="n">
-        <v>52</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -813,17 +809,13 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="n">
-        <v>6</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
+      <c r="C3"/>
+      <c r="D3"/>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -834,19 +826,15 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4"/>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -859,14 +847,10 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
+      <c r="C5"/>
+      <c r="D5"/>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -882,17 +866,13 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
+      <c r="C6"/>
+      <c r="D6"/>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -905,17 +885,13 @@
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
+      <c r="C7"/>
+      <c r="D7"/>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
@@ -928,14 +904,10 @@
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8" t="n">
         <v>2</v>
-      </c>
-      <c r="D8" t="n">
-        <v>3</v>
-      </c>
-      <c r="E8" t="n">
-        <v>5</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
@@ -951,12 +923,8 @@
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2</v>
-      </c>
+      <c r="C9"/>
+      <c r="D9"/>
       <c r="E9" t="n">
         <v>3</v>
       </c>
@@ -974,14 +942,10 @@
       <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="n">
-        <v>8</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
+      <c r="C10"/>
+      <c r="D10"/>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -997,14 +961,10 @@
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
+      <c r="C11"/>
+      <c r="D11"/>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -1020,14 +980,10 @@
       <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="n">
-        <v>15</v>
-      </c>
-      <c r="D12" t="n">
-        <v>29</v>
-      </c>
+      <c r="C12"/>
+      <c r="D12"/>
       <c r="E12" t="n">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
@@ -1043,12 +999,8 @@
       <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
+      <c r="C13"/>
+      <c r="D13"/>
       <c r="E13" t="n">
         <v>1</v>
       </c>
@@ -1066,14 +1018,10 @@
       <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="n">
-        <v>3</v>
-      </c>
-      <c r="D14" t="n">
-        <v>18</v>
-      </c>
+      <c r="C14"/>
+      <c r="D14"/>
       <c r="E14" t="n">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
         <v>9</v>
@@ -1089,14 +1037,10 @@
       <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C15" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" t="n">
-        <v>5</v>
-      </c>
+      <c r="C15"/>
+      <c r="D15"/>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
@@ -1112,20 +1056,16 @@
       <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="C16" t="n">
-        <v>4</v>
-      </c>
-      <c r="D16" t="n">
-        <v>6</v>
-      </c>
+      <c r="C16"/>
+      <c r="D16"/>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F16" t="s">
         <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
@@ -1135,14 +1075,10 @@
       <c r="B17" t="s">
         <v>25</v>
       </c>
-      <c r="C17" t="n">
-        <v>8</v>
-      </c>
-      <c r="D17" t="n">
-        <v>3</v>
-      </c>
+      <c r="C17"/>
+      <c r="D17"/>
       <c r="E17" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F17" t="s">
         <v>9</v>
@@ -1158,20 +1094,16 @@
       <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>3</v>
-      </c>
+      <c r="C18"/>
+      <c r="D18"/>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
         <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
@@ -1181,14 +1113,10 @@
       <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1</v>
-      </c>
+      <c r="C19"/>
+      <c r="D19"/>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F19" t="s">
         <v>9</v>
@@ -1204,14 +1132,10 @@
       <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="C20" t="n">
-        <v>79</v>
-      </c>
-      <c r="D20" t="n">
-        <v>41</v>
-      </c>
+      <c r="C20"/>
+      <c r="D20"/>
       <c r="E20" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="F20" t="s">
         <v>9</v>
@@ -1227,14 +1151,10 @@
       <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="C21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" t="n">
-        <v>3</v>
-      </c>
+      <c r="C21"/>
+      <c r="D21"/>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
         <v>9</v>
@@ -1250,14 +1170,10 @@
       <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
+      <c r="C22"/>
+      <c r="D22"/>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F22" t="s">
         <v>9</v>
@@ -1273,17 +1189,13 @@
       <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="C23" t="n">
-        <v>8</v>
-      </c>
-      <c r="D23" t="n">
-        <v>35</v>
-      </c>
+      <c r="C23"/>
+      <c r="D23"/>
       <c r="E23" t="n">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G23" t="s">
         <v>9</v>
@@ -1296,17 +1208,13 @@
       <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>1</v>
-      </c>
+      <c r="C24"/>
+      <c r="D24"/>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
         <v>9</v>
@@ -1319,17 +1227,13 @@
       <c r="B25" t="s">
         <v>33</v>
       </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>1</v>
-      </c>
+      <c r="C25"/>
+      <c r="D25"/>
       <c r="E25" t="n">
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
         <v>9</v>
@@ -1342,17 +1246,13 @@
       <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="C26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" t="n">
-        <v>1</v>
-      </c>
+      <c r="C26"/>
+      <c r="D26"/>
       <c r="E26" t="n">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
         <v>9</v>
@@ -1365,17 +1265,13 @@
       <c r="B27" t="s">
         <v>35</v>
       </c>
-      <c r="C27" t="n">
-        <v>27</v>
-      </c>
-      <c r="D27" t="n">
-        <v>56</v>
-      </c>
+      <c r="C27"/>
+      <c r="D27"/>
       <c r="E27" t="n">
-        <v>83</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
         <v>9</v>
@@ -1388,17 +1284,13 @@
       <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="C28" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" t="n">
-        <v>1</v>
-      </c>
+      <c r="C28"/>
+      <c r="D28"/>
       <c r="E28" t="n">
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s">
         <v>9</v>
@@ -1411,17 +1303,13 @@
       <c r="B29" t="s">
         <v>37</v>
       </c>
-      <c r="C29" t="n">
-        <v>11</v>
-      </c>
-      <c r="D29" t="n">
-        <v>14</v>
-      </c>
+      <c r="C29"/>
+      <c r="D29"/>
       <c r="E29" t="n">
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
         <v>9</v>
@@ -1434,12 +1322,8 @@
       <c r="B30" t="s">
         <v>38</v>
       </c>
-      <c r="C30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" t="n">
-        <v>1</v>
-      </c>
+      <c r="C30"/>
+      <c r="D30"/>
       <c r="E30" t="n">
         <v>1</v>
       </c>
@@ -1457,12 +1341,8 @@
       <c r="B31" t="s">
         <v>39</v>
       </c>
-      <c r="C31" t="n">
-        <v>6</v>
-      </c>
-      <c r="D31" t="n">
-        <v>1</v>
-      </c>
+      <c r="C31"/>
+      <c r="D31"/>
       <c r="E31" t="n">
         <v>7</v>
       </c>
@@ -1480,20 +1360,16 @@
       <c r="B32" t="s">
         <v>41</v>
       </c>
-      <c r="C32" t="n">
-        <v>10</v>
-      </c>
-      <c r="D32" t="n">
-        <v>1</v>
-      </c>
+      <c r="C32"/>
+      <c r="D32"/>
       <c r="E32" t="n">
         <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33">
@@ -1503,20 +1379,16 @@
       <c r="B33" t="s">
         <v>42</v>
       </c>
-      <c r="C33" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
+      <c r="C33"/>
+      <c r="D33"/>
       <c r="E33" t="n">
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34">
@@ -1526,17 +1398,13 @@
       <c r="B34" t="s">
         <v>43</v>
       </c>
-      <c r="C34" t="n">
-        <v>8</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0</v>
-      </c>
+      <c r="C34"/>
+      <c r="D34"/>
       <c r="E34" t="n">
         <v>8</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
         <v>9</v>
@@ -1549,20 +1417,16 @@
       <c r="B35" t="s">
         <v>44</v>
       </c>
-      <c r="C35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" t="n">
-        <v>1</v>
-      </c>
+      <c r="C35"/>
+      <c r="D35"/>
       <c r="E35" t="n">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36">
@@ -1572,20 +1436,16 @@
       <c r="B36" t="s">
         <v>45</v>
       </c>
-      <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" t="n">
-        <v>1</v>
-      </c>
+      <c r="C36"/>
+      <c r="D36"/>
       <c r="E36" t="n">
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37">
@@ -1595,20 +1455,16 @@
       <c r="B37" t="s">
         <v>46</v>
       </c>
-      <c r="C37" t="n">
-        <v>2</v>
-      </c>
-      <c r="D37" t="n">
-        <v>14</v>
-      </c>
+      <c r="C37"/>
+      <c r="D37"/>
       <c r="E37" t="n">
         <v>16</v>
       </c>
       <c r="F37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38">
@@ -1618,17 +1474,13 @@
       <c r="B38" t="s">
         <v>47</v>
       </c>
-      <c r="C38" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0</v>
-      </c>
+      <c r="C38"/>
+      <c r="D38"/>
       <c r="E38" t="n">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G38" t="s">
         <v>9</v>
@@ -1641,17 +1493,13 @@
       <c r="B39" t="s">
         <v>48</v>
       </c>
-      <c r="C39" t="n">
-        <v>1</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0</v>
-      </c>
+      <c r="C39"/>
+      <c r="D39"/>
       <c r="E39" t="n">
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s">
         <v>9</v>
@@ -1664,17 +1512,13 @@
       <c r="B40" t="s">
         <v>49</v>
       </c>
-      <c r="C40" t="n">
-        <v>9</v>
-      </c>
-      <c r="D40" t="n">
-        <v>22</v>
-      </c>
+      <c r="C40"/>
+      <c r="D40"/>
       <c r="E40" t="n">
         <v>31</v>
       </c>
       <c r="F40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G40" t="s">
         <v>9</v>
@@ -1687,20 +1531,16 @@
       <c r="B41" t="s">
         <v>50</v>
       </c>
-      <c r="C41" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" t="n">
-        <v>2</v>
-      </c>
+      <c r="C41"/>
+      <c r="D41"/>
       <c r="E41" t="n">
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42">
@@ -1710,17 +1550,13 @@
       <c r="B42" t="s">
         <v>51</v>
       </c>
-      <c r="C42" t="n">
-        <v>2</v>
-      </c>
-      <c r="D42" t="n">
-        <v>6</v>
-      </c>
+      <c r="C42"/>
+      <c r="D42"/>
       <c r="E42" t="n">
         <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G42" t="s">
         <v>9</v>
@@ -1733,17 +1569,13 @@
       <c r="B43" t="s">
         <v>52</v>
       </c>
-      <c r="C43" t="n">
-        <v>2</v>
-      </c>
-      <c r="D43" t="n">
-        <v>2</v>
-      </c>
+      <c r="C43"/>
+      <c r="D43"/>
       <c r="E43" t="n">
         <v>4</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G43" t="s">
         <v>9</v>
@@ -1756,17 +1588,13 @@
       <c r="B44" t="s">
         <v>53</v>
       </c>
-      <c r="C44" t="n">
-        <v>1</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0</v>
-      </c>
+      <c r="C44"/>
+      <c r="D44"/>
       <c r="E44" t="n">
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G44" t="s">
         <v>9</v>
@@ -1779,17 +1607,13 @@
       <c r="B45" t="s">
         <v>54</v>
       </c>
-      <c r="C45" t="n">
-        <v>1</v>
-      </c>
-      <c r="D45" t="n">
-        <v>0</v>
-      </c>
+      <c r="C45"/>
+      <c r="D45"/>
       <c r="E45" t="n">
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G45" t="s">
         <v>9</v>
@@ -1802,20 +1626,16 @@
       <c r="B46" t="s">
         <v>55</v>
       </c>
-      <c r="C46" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" t="n">
-        <v>1</v>
-      </c>
+      <c r="C46"/>
+      <c r="D46"/>
       <c r="E46" t="n">
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47">
@@ -1825,17 +1645,13 @@
       <c r="B47" t="s">
         <v>56</v>
       </c>
-      <c r="C47" t="n">
-        <v>1</v>
-      </c>
-      <c r="D47" t="n">
-        <v>0</v>
-      </c>
+      <c r="C47"/>
+      <c r="D47"/>
       <c r="E47" t="n">
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s">
         <v>9</v>
@@ -1848,20 +1664,16 @@
       <c r="B48" t="s">
         <v>57</v>
       </c>
-      <c r="C48" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" t="n">
-        <v>0</v>
-      </c>
+      <c r="C48"/>
+      <c r="D48"/>
       <c r="E48" t="n">
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49">
@@ -1871,17 +1683,13 @@
       <c r="B49" t="s">
         <v>58</v>
       </c>
-      <c r="C49" t="n">
-        <v>4</v>
-      </c>
-      <c r="D49" t="n">
-        <v>1</v>
-      </c>
+      <c r="C49"/>
+      <c r="D49"/>
       <c r="E49" t="n">
         <v>5</v>
       </c>
       <c r="F49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G49" t="s">
         <v>9</v>
@@ -1894,20 +1702,16 @@
       <c r="B50" t="s">
         <v>59</v>
       </c>
-      <c r="C50" t="n">
-        <v>3</v>
-      </c>
-      <c r="D50" t="n">
-        <v>3</v>
-      </c>
+      <c r="C50"/>
+      <c r="D50"/>
       <c r="E50" t="n">
         <v>6</v>
       </c>
       <c r="F50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51">
@@ -1917,20 +1721,16 @@
       <c r="B51" t="s">
         <v>60</v>
       </c>
-      <c r="C51" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" t="n">
-        <v>1</v>
-      </c>
+      <c r="C51"/>
+      <c r="D51"/>
       <c r="E51" t="n">
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52">
@@ -1940,20 +1740,16 @@
       <c r="B52" t="s">
         <v>61</v>
       </c>
-      <c r="C52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D52" t="n">
-        <v>1</v>
-      </c>
+      <c r="C52"/>
+      <c r="D52"/>
       <c r="E52" t="n">
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53">
@@ -1963,20 +1759,16 @@
       <c r="B53" t="s">
         <v>62</v>
       </c>
-      <c r="C53" t="n">
-        <v>28</v>
-      </c>
-      <c r="D53" t="n">
-        <v>14</v>
-      </c>
+      <c r="C53"/>
+      <c r="D53"/>
       <c r="E53" t="n">
         <v>42</v>
       </c>
       <c r="F53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54">
@@ -1986,20 +1778,16 @@
       <c r="B54" t="s">
         <v>63</v>
       </c>
-      <c r="C54" t="n">
-        <v>22</v>
-      </c>
-      <c r="D54" t="n">
-        <v>64</v>
-      </c>
+      <c r="C54"/>
+      <c r="D54"/>
       <c r="E54" t="n">
         <v>86</v>
       </c>
       <c r="F54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55">
@@ -2009,17 +1797,13 @@
       <c r="B55" t="s">
         <v>64</v>
       </c>
-      <c r="C55" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" t="n">
-        <v>1</v>
-      </c>
+      <c r="C55"/>
+      <c r="D55"/>
       <c r="E55" t="n">
         <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G55" t="s">
         <v>9</v>
@@ -2032,20 +1816,16 @@
       <c r="B56" t="s">
         <v>65</v>
       </c>
-      <c r="C56" t="n">
-        <v>3</v>
-      </c>
-      <c r="D56" t="n">
-        <v>7</v>
-      </c>
+      <c r="C56"/>
+      <c r="D56"/>
       <c r="E56" t="n">
         <v>10</v>
       </c>
       <c r="F56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57">
@@ -2055,17 +1835,13 @@
       <c r="B57" t="s">
         <v>66</v>
       </c>
-      <c r="C57" t="n">
-        <v>2</v>
-      </c>
-      <c r="D57" t="n">
-        <v>1</v>
-      </c>
+      <c r="C57"/>
+      <c r="D57"/>
       <c r="E57" t="n">
         <v>3</v>
       </c>
       <c r="F57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G57" t="s">
         <v>9</v>
@@ -2078,20 +1854,16 @@
       <c r="B58" t="s">
         <v>67</v>
       </c>
-      <c r="C58" t="n">
-        <v>1</v>
-      </c>
-      <c r="D58" t="n">
-        <v>6</v>
-      </c>
+      <c r="C58"/>
+      <c r="D58"/>
       <c r="E58" t="n">
         <v>7</v>
       </c>
       <c r="F58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59">
@@ -2101,20 +1873,16 @@
       <c r="B59" t="s">
         <v>68</v>
       </c>
-      <c r="C59" t="n">
-        <v>0</v>
-      </c>
-      <c r="D59" t="n">
-        <v>3</v>
-      </c>
+      <c r="C59"/>
+      <c r="D59"/>
       <c r="E59" t="n">
         <v>3</v>
       </c>
       <c r="F59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60">
@@ -2124,12 +1892,8 @@
       <c r="B60" t="s">
         <v>69</v>
       </c>
-      <c r="C60" t="n">
-        <v>3</v>
-      </c>
-      <c r="D60" t="n">
-        <v>0</v>
-      </c>
+      <c r="C60"/>
+      <c r="D60"/>
       <c r="E60" t="n">
         <v>3</v>
       </c>
@@ -2147,12 +1911,8 @@
       <c r="B61" t="s">
         <v>70</v>
       </c>
-      <c r="C61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D61" t="n">
-        <v>3</v>
-      </c>
+      <c r="C61"/>
+      <c r="D61"/>
       <c r="E61" t="n">
         <v>3</v>
       </c>
@@ -2160,7 +1920,7 @@
         <v>9</v>
       </c>
       <c r="G61" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62">
@@ -2170,20 +1930,16 @@
       <c r="B62" t="s">
         <v>71</v>
       </c>
-      <c r="C62" t="n">
-        <v>2</v>
-      </c>
-      <c r="D62" t="n">
-        <v>1</v>
-      </c>
+      <c r="C62"/>
+      <c r="D62"/>
       <c r="E62" t="n">
         <v>3</v>
       </c>
       <c r="F62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63">
@@ -2193,17 +1949,13 @@
       <c r="B63" t="s">
         <v>72</v>
       </c>
-      <c r="C63" t="n">
-        <v>1</v>
-      </c>
-      <c r="D63" t="n">
-        <v>0</v>
-      </c>
+      <c r="C63"/>
+      <c r="D63"/>
       <c r="E63" t="n">
         <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G63" t="s">
         <v>9</v>
@@ -2216,20 +1968,16 @@
       <c r="B64" t="s">
         <v>73</v>
       </c>
-      <c r="C64" t="n">
-        <v>3</v>
-      </c>
-      <c r="D64" t="n">
-        <v>10</v>
-      </c>
+      <c r="C64"/>
+      <c r="D64"/>
       <c r="E64" t="n">
         <v>13</v>
       </c>
       <c r="F64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65">
@@ -2239,20 +1987,16 @@
       <c r="B65" t="s">
         <v>74</v>
       </c>
-      <c r="C65" t="n">
-        <v>32</v>
-      </c>
-      <c r="D65" t="n">
-        <v>8</v>
-      </c>
+      <c r="C65"/>
+      <c r="D65"/>
       <c r="E65" t="n">
         <v>40</v>
       </c>
       <c r="F65" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66">
@@ -2262,20 +2006,16 @@
       <c r="B66" t="s">
         <v>75</v>
       </c>
-      <c r="C66" t="n">
-        <v>4</v>
-      </c>
-      <c r="D66" t="n">
-        <v>1</v>
-      </c>
+      <c r="C66"/>
+      <c r="D66"/>
       <c r="E66" t="n">
         <v>5</v>
       </c>
       <c r="F66" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G66" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67">
@@ -2285,20 +2025,16 @@
       <c r="B67" t="s">
         <v>76</v>
       </c>
-      <c r="C67" t="n">
-        <v>352</v>
-      </c>
-      <c r="D67" t="n">
-        <v>470</v>
-      </c>
+      <c r="C67"/>
+      <c r="D67"/>
       <c r="E67" t="n">
         <v>822</v>
       </c>
       <c r="F67" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G67" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68">
@@ -2308,20 +2044,16 @@
       <c r="B68" t="s">
         <v>77</v>
       </c>
-      <c r="C68" t="n">
-        <v>154</v>
-      </c>
-      <c r="D68" t="n">
-        <v>230</v>
-      </c>
+      <c r="C68"/>
+      <c r="D68"/>
       <c r="E68" t="n">
         <v>384</v>
       </c>
       <c r="F68" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G68" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69">
@@ -2332,10 +2064,10 @@
         <v>79</v>
       </c>
       <c r="C69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" t="n">
         <v>0</v>
-      </c>
-      <c r="D69" t="n">
-        <v>1</v>
       </c>
       <c r="E69" t="n">
         <v>1</v>
@@ -2354,14 +2086,10 @@
       <c r="B70" t="s">
         <v>80</v>
       </c>
-      <c r="C70" t="n">
-        <v>2</v>
-      </c>
-      <c r="D70" t="n">
-        <v>2</v>
-      </c>
+      <c r="C70"/>
+      <c r="D70"/>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F70" t="s">
         <v>9</v>
@@ -2377,20 +2105,16 @@
       <c r="B71" t="s">
         <v>81</v>
       </c>
-      <c r="C71" t="n">
-        <v>2</v>
-      </c>
-      <c r="D71" t="n">
+      <c r="C71"/>
+      <c r="D71"/>
+      <c r="E71" t="n">
         <v>4</v>
       </c>
-      <c r="E71" t="n">
-        <v>6</v>
-      </c>
       <c r="F71" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G71" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72">
@@ -2400,20 +2124,16 @@
       <c r="B72" t="s">
         <v>82</v>
       </c>
-      <c r="C72" t="n">
-        <v>0</v>
-      </c>
-      <c r="D72" t="n">
-        <v>1</v>
-      </c>
+      <c r="C72"/>
+      <c r="D72"/>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F72" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G72" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73">
@@ -2423,20 +2143,16 @@
       <c r="B73" t="s">
         <v>83</v>
       </c>
-      <c r="C73" t="n">
-        <v>28</v>
-      </c>
-      <c r="D73" t="n">
-        <v>16</v>
-      </c>
+      <c r="C73"/>
+      <c r="D73"/>
       <c r="E73" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F73" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G73" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74">
@@ -2446,20 +2162,16 @@
       <c r="B74" t="s">
         <v>84</v>
       </c>
-      <c r="C74" t="n">
-        <v>2</v>
-      </c>
-      <c r="D74" t="n">
-        <v>6</v>
-      </c>
+      <c r="C74"/>
+      <c r="D74"/>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="F74" t="s">
         <v>9</v>
       </c>
       <c r="G74" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75">
@@ -2469,20 +2181,16 @@
       <c r="B75" t="s">
         <v>85</v>
       </c>
-      <c r="C75" t="n">
-        <v>1</v>
-      </c>
-      <c r="D75" t="n">
-        <v>3</v>
-      </c>
+      <c r="C75"/>
+      <c r="D75"/>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F75" t="s">
         <v>9</v>
       </c>
       <c r="G75" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76">
@@ -2492,20 +2200,16 @@
       <c r="B76" t="s">
         <v>86</v>
       </c>
-      <c r="C76" t="n">
-        <v>14</v>
-      </c>
-      <c r="D76" t="n">
-        <v>40</v>
-      </c>
+      <c r="C76"/>
+      <c r="D76"/>
       <c r="E76" t="n">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="F76" t="s">
         <v>9</v>
       </c>
       <c r="G76" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77">
@@ -2515,20 +2219,16 @@
       <c r="B77" t="s">
         <v>87</v>
       </c>
-      <c r="C77" t="n">
-        <v>3</v>
-      </c>
-      <c r="D77" t="n">
-        <v>0</v>
-      </c>
+      <c r="C77"/>
+      <c r="D77"/>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="F77" t="s">
         <v>9</v>
       </c>
       <c r="G77" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78">
@@ -2538,14 +2238,10 @@
       <c r="B78" t="s">
         <v>88</v>
       </c>
-      <c r="C78" t="n">
-        <v>6</v>
-      </c>
-      <c r="D78" t="n">
-        <v>22</v>
-      </c>
+      <c r="C78"/>
+      <c r="D78"/>
       <c r="E78" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="F78" t="s">
         <v>9</v>
@@ -2561,14 +2257,10 @@
       <c r="B79" t="s">
         <v>89</v>
       </c>
-      <c r="C79" t="n">
-        <v>1</v>
-      </c>
-      <c r="D79" t="n">
-        <v>0</v>
-      </c>
+      <c r="C79"/>
+      <c r="D79"/>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F79" t="s">
         <v>9</v>
@@ -2584,17 +2276,13 @@
       <c r="B80" t="s">
         <v>90</v>
       </c>
-      <c r="C80" t="n">
-        <v>0</v>
-      </c>
-      <c r="D80" t="n">
-        <v>1</v>
-      </c>
+      <c r="C80"/>
+      <c r="D80"/>
       <c r="E80" t="n">
         <v>1</v>
       </c>
       <c r="F80" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G80" t="s">
         <v>9</v>
@@ -2607,12 +2295,8 @@
       <c r="B81" t="s">
         <v>91</v>
       </c>
-      <c r="C81" t="n">
-        <v>11</v>
-      </c>
-      <c r="D81" t="n">
-        <v>0</v>
-      </c>
+      <c r="C81"/>
+      <c r="D81"/>
       <c r="E81" t="n">
         <v>11</v>
       </c>
@@ -2620,7 +2304,7 @@
         <v>9</v>
       </c>
       <c r="G81" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82">
@@ -2630,17 +2314,13 @@
       <c r="B82" t="s">
         <v>92</v>
       </c>
-      <c r="C82" t="n">
-        <v>0</v>
-      </c>
-      <c r="D82" t="n">
-        <v>98</v>
-      </c>
+      <c r="C82"/>
+      <c r="D82"/>
       <c r="E82" t="n">
         <v>98</v>
       </c>
       <c r="F82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G82" t="s">
         <v>9</v>
@@ -2653,17 +2333,13 @@
       <c r="B83" t="s">
         <v>93</v>
       </c>
-      <c r="C83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D83" t="n">
-        <v>4</v>
-      </c>
+      <c r="C83"/>
+      <c r="D83"/>
       <c r="E83" t="n">
         <v>4</v>
       </c>
       <c r="F83" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G83" t="s">
         <v>9</v>
@@ -2676,17 +2352,13 @@
       <c r="B84" t="s">
         <v>94</v>
       </c>
-      <c r="C84" t="n">
-        <v>0</v>
-      </c>
-      <c r="D84" t="n">
-        <v>1</v>
-      </c>
+      <c r="C84"/>
+      <c r="D84"/>
       <c r="E84" t="n">
         <v>1</v>
       </c>
       <c r="F84" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G84" t="s">
         <v>9</v>
@@ -2699,12 +2371,8 @@
       <c r="B85" t="s">
         <v>95</v>
       </c>
-      <c r="C85" t="n">
-        <v>7</v>
-      </c>
-      <c r="D85" t="n">
-        <v>154</v>
-      </c>
+      <c r="C85"/>
+      <c r="D85"/>
       <c r="E85" t="n">
         <v>161</v>
       </c>
@@ -2722,20 +2390,16 @@
       <c r="B86" t="s">
         <v>96</v>
       </c>
-      <c r="C86" t="n">
-        <v>0</v>
-      </c>
-      <c r="D86" t="n">
-        <v>1</v>
-      </c>
+      <c r="C86"/>
+      <c r="D86"/>
       <c r="E86" t="n">
         <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G86" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87">
@@ -2745,20 +2409,16 @@
       <c r="B87" t="s">
         <v>97</v>
       </c>
-      <c r="C87" t="n">
-        <v>6</v>
-      </c>
-      <c r="D87" t="n">
-        <v>6</v>
-      </c>
+      <c r="C87"/>
+      <c r="D87"/>
       <c r="E87" t="n">
         <v>12</v>
       </c>
       <c r="F87" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G87" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88">
@@ -2768,12 +2428,8 @@
       <c r="B88" t="s">
         <v>98</v>
       </c>
-      <c r="C88" t="n">
-        <v>16</v>
-      </c>
-      <c r="D88" t="n">
-        <v>142</v>
-      </c>
+      <c r="C88"/>
+      <c r="D88"/>
       <c r="E88" t="n">
         <v>158</v>
       </c>
@@ -2791,12 +2447,8 @@
       <c r="B89" t="s">
         <v>99</v>
       </c>
-      <c r="C89" t="n">
-        <v>1</v>
-      </c>
-      <c r="D89" t="n">
-        <v>0</v>
-      </c>
+      <c r="C89"/>
+      <c r="D89"/>
       <c r="E89" t="n">
         <v>1</v>
       </c>
@@ -2814,12 +2466,8 @@
       <c r="B90" t="s">
         <v>100</v>
       </c>
-      <c r="C90" t="n">
-        <v>20</v>
-      </c>
-      <c r="D90" t="n">
-        <v>7</v>
-      </c>
+      <c r="C90"/>
+      <c r="D90"/>
       <c r="E90" t="n">
         <v>27</v>
       </c>
@@ -2827,7 +2475,7 @@
         <v>9</v>
       </c>
       <c r="G90" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91">
@@ -2837,17 +2485,13 @@
       <c r="B91" t="s">
         <v>101</v>
       </c>
-      <c r="C91" t="n">
-        <v>36</v>
-      </c>
-      <c r="D91" t="n">
-        <v>7</v>
-      </c>
+      <c r="C91"/>
+      <c r="D91"/>
       <c r="E91" t="n">
         <v>43</v>
       </c>
       <c r="F91" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G91" t="s">
         <v>9</v>
@@ -2860,12 +2504,8 @@
       <c r="B92" t="s">
         <v>102</v>
       </c>
-      <c r="C92" t="n">
-        <v>59</v>
-      </c>
-      <c r="D92" t="n">
-        <v>43</v>
-      </c>
+      <c r="C92"/>
+      <c r="D92"/>
       <c r="E92" t="n">
         <v>102</v>
       </c>
@@ -2883,12 +2523,8 @@
       <c r="B93" t="s">
         <v>103</v>
       </c>
-      <c r="C93" t="n">
-        <v>54</v>
-      </c>
-      <c r="D93" t="n">
-        <v>15</v>
-      </c>
+      <c r="C93"/>
+      <c r="D93"/>
       <c r="E93" t="n">
         <v>69</v>
       </c>
@@ -2906,12 +2542,8 @@
       <c r="B94" t="s">
         <v>104</v>
       </c>
-      <c r="C94" t="n">
-        <v>122</v>
-      </c>
-      <c r="D94" t="n">
-        <v>228</v>
-      </c>
+      <c r="C94"/>
+      <c r="D94"/>
       <c r="E94" t="n">
         <v>350</v>
       </c>
@@ -2929,12 +2561,8 @@
       <c r="B95" t="s">
         <v>105</v>
       </c>
-      <c r="C95" t="n">
-        <v>1</v>
-      </c>
-      <c r="D95" t="n">
-        <v>0</v>
-      </c>
+      <c r="C95"/>
+      <c r="D95"/>
       <c r="E95" t="n">
         <v>1</v>
       </c>
@@ -2952,12 +2580,8 @@
       <c r="B96" t="s">
         <v>106</v>
       </c>
-      <c r="C96" t="n">
-        <v>4</v>
-      </c>
-      <c r="D96" t="n">
-        <v>1</v>
-      </c>
+      <c r="C96"/>
+      <c r="D96"/>
       <c r="E96" t="n">
         <v>5</v>
       </c>
@@ -2965,7 +2589,7 @@
         <v>9</v>
       </c>
       <c r="G96" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97">
@@ -2975,12 +2599,8 @@
       <c r="B97" t="s">
         <v>107</v>
       </c>
-      <c r="C97" t="n">
-        <v>16</v>
-      </c>
-      <c r="D97" t="n">
-        <v>1</v>
-      </c>
+      <c r="C97"/>
+      <c r="D97"/>
       <c r="E97" t="n">
         <v>17</v>
       </c>
@@ -2988,7 +2608,7 @@
         <v>9</v>
       </c>
       <c r="G97" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98">
@@ -2998,12 +2618,8 @@
       <c r="B98" t="s">
         <v>108</v>
       </c>
-      <c r="C98" t="n">
-        <v>1</v>
-      </c>
-      <c r="D98" t="n">
-        <v>1</v>
-      </c>
+      <c r="C98"/>
+      <c r="D98"/>
       <c r="E98" t="n">
         <v>2</v>
       </c>
@@ -3011,7 +2627,7 @@
         <v>9</v>
       </c>
       <c r="G98" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99">
@@ -3021,12 +2637,8 @@
       <c r="B99" t="s">
         <v>109</v>
       </c>
-      <c r="C99" t="n">
-        <v>1</v>
-      </c>
-      <c r="D99" t="n">
-        <v>1</v>
-      </c>
+      <c r="C99"/>
+      <c r="D99"/>
       <c r="E99" t="n">
         <v>2</v>
       </c>
@@ -3034,7 +2646,7 @@
         <v>9</v>
       </c>
       <c r="G99" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100">
@@ -3044,20 +2656,16 @@
       <c r="B100" t="s">
         <v>110</v>
       </c>
-      <c r="C100" t="n">
-        <v>3</v>
-      </c>
-      <c r="D100" t="n">
-        <v>14</v>
-      </c>
+      <c r="C100"/>
+      <c r="D100"/>
       <c r="E100" t="n">
         <v>17</v>
       </c>
       <c r="F100" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G100" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101">
@@ -3067,12 +2675,8 @@
       <c r="B101" t="s">
         <v>111</v>
       </c>
-      <c r="C101" t="n">
-        <v>0</v>
-      </c>
-      <c r="D101" t="n">
-        <v>1</v>
-      </c>
+      <c r="C101"/>
+      <c r="D101"/>
       <c r="E101" t="n">
         <v>1</v>
       </c>
@@ -3090,12 +2694,8 @@
       <c r="B102" t="s">
         <v>112</v>
       </c>
-      <c r="C102" t="n">
-        <v>0</v>
-      </c>
-      <c r="D102" t="n">
-        <v>2</v>
-      </c>
+      <c r="C102"/>
+      <c r="D102"/>
       <c r="E102" t="n">
         <v>2</v>
       </c>
@@ -3113,12 +2713,8 @@
       <c r="B103" t="s">
         <v>113</v>
       </c>
-      <c r="C103" t="n">
-        <v>4</v>
-      </c>
-      <c r="D103" t="n">
-        <v>1</v>
-      </c>
+      <c r="C103"/>
+      <c r="D103"/>
       <c r="E103" t="n">
         <v>5</v>
       </c>
@@ -3136,12 +2732,8 @@
       <c r="B104" t="s">
         <v>114</v>
       </c>
-      <c r="C104" t="n">
-        <v>0</v>
-      </c>
-      <c r="D104" t="n">
-        <v>1</v>
-      </c>
+      <c r="C104"/>
+      <c r="D104"/>
       <c r="E104" t="n">
         <v>1</v>
       </c>
@@ -3159,12 +2751,8 @@
       <c r="B105" t="s">
         <v>115</v>
       </c>
-      <c r="C105" t="n">
-        <v>13</v>
-      </c>
-      <c r="D105" t="n">
-        <v>8</v>
-      </c>
+      <c r="C105"/>
+      <c r="D105"/>
       <c r="E105" t="n">
         <v>21</v>
       </c>
@@ -3182,20 +2770,16 @@
       <c r="B106" t="s">
         <v>117</v>
       </c>
-      <c r="C106" t="n">
-        <v>2</v>
-      </c>
-      <c r="D106" t="n">
-        <v>2</v>
-      </c>
+      <c r="C106"/>
+      <c r="D106"/>
       <c r="E106" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F106" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G106" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107">
@@ -3205,20 +2789,16 @@
       <c r="B107" t="s">
         <v>118</v>
       </c>
-      <c r="C107" t="n">
-        <v>3</v>
-      </c>
-      <c r="D107" t="n">
-        <v>1</v>
-      </c>
+      <c r="C107"/>
+      <c r="D107"/>
       <c r="E107" t="n">
         <v>4</v>
       </c>
       <c r="F107" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G107" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108">
@@ -3228,12 +2808,8 @@
       <c r="B108" t="s">
         <v>119</v>
       </c>
-      <c r="C108" t="n">
-        <v>0</v>
-      </c>
-      <c r="D108" t="n">
-        <v>4</v>
-      </c>
+      <c r="C108"/>
+      <c r="D108"/>
       <c r="E108" t="n">
         <v>4</v>
       </c>
@@ -3241,7 +2817,7 @@
         <v>9</v>
       </c>
       <c r="G108" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109">
@@ -3251,20 +2827,16 @@
       <c r="B109" t="s">
         <v>120</v>
       </c>
-      <c r="C109" t="n">
-        <v>2</v>
-      </c>
-      <c r="D109" t="n">
-        <v>1</v>
-      </c>
+      <c r="C109"/>
+      <c r="D109"/>
       <c r="E109" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F109" t="s">
         <v>9</v>
       </c>
       <c r="G109" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110">
@@ -3274,17 +2846,13 @@
       <c r="B110" t="s">
         <v>121</v>
       </c>
-      <c r="C110" t="n">
-        <v>1</v>
-      </c>
-      <c r="D110" t="n">
-        <v>11</v>
-      </c>
+      <c r="C110"/>
+      <c r="D110"/>
       <c r="E110" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F110" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G110" t="s">
         <v>9</v>
@@ -3297,17 +2865,13 @@
       <c r="B111" t="s">
         <v>122</v>
       </c>
-      <c r="C111" t="n">
-        <v>1</v>
-      </c>
-      <c r="D111" t="n">
-        <v>3</v>
-      </c>
+      <c r="C111"/>
+      <c r="D111"/>
       <c r="E111" t="n">
         <v>4</v>
       </c>
       <c r="F111" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G111" t="s">
         <v>9</v>
@@ -3320,12 +2884,8 @@
       <c r="B112" t="s">
         <v>123</v>
       </c>
-      <c r="C112" t="n">
-        <v>25</v>
-      </c>
-      <c r="D112" t="n">
-        <v>4</v>
-      </c>
+      <c r="C112"/>
+      <c r="D112"/>
       <c r="E112" t="n">
         <v>29</v>
       </c>
@@ -3343,20 +2903,16 @@
       <c r="B113" t="s">
         <v>125</v>
       </c>
-      <c r="C113" t="n">
-        <v>43</v>
-      </c>
-      <c r="D113" t="n">
-        <v>96</v>
-      </c>
+      <c r="C113"/>
+      <c r="D113"/>
       <c r="E113" t="n">
-        <v>139</v>
+        <v>3</v>
       </c>
       <c r="F113" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G113" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114">
@@ -3366,20 +2922,16 @@
       <c r="B114" t="s">
         <v>126</v>
       </c>
-      <c r="C114" t="n">
-        <v>3</v>
-      </c>
-      <c r="D114" t="n">
-        <v>5</v>
-      </c>
+      <c r="C114"/>
+      <c r="D114"/>
       <c r="E114" t="n">
-        <v>8</v>
+        <v>139</v>
       </c>
       <c r="F114" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G114" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115">
@@ -3389,20 +2941,16 @@
       <c r="B115" t="s">
         <v>127</v>
       </c>
-      <c r="C115" t="n">
-        <v>0</v>
-      </c>
-      <c r="D115" t="n">
-        <v>1</v>
-      </c>
+      <c r="C115"/>
+      <c r="D115"/>
       <c r="E115" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F115" t="s">
         <v>9</v>
       </c>
       <c r="G115" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116">
@@ -3412,17 +2960,13 @@
       <c r="B116" t="s">
         <v>128</v>
       </c>
-      <c r="C116" t="n">
-        <v>1</v>
-      </c>
-      <c r="D116" t="n">
-        <v>3</v>
-      </c>
+      <c r="C116"/>
+      <c r="D116"/>
       <c r="E116" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F116" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G116" t="s">
         <v>9</v>
@@ -3435,20 +2979,16 @@
       <c r="B117" t="s">
         <v>129</v>
       </c>
-      <c r="C117" t="n">
-        <v>5</v>
-      </c>
-      <c r="D117" t="n">
-        <v>20</v>
-      </c>
+      <c r="C117"/>
+      <c r="D117"/>
       <c r="E117" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F117" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G117" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="118">
@@ -3458,20 +2998,16 @@
       <c r="B118" t="s">
         <v>130</v>
       </c>
-      <c r="C118" t="n">
-        <v>1</v>
-      </c>
-      <c r="D118" t="n">
-        <v>10</v>
-      </c>
+      <c r="C118"/>
+      <c r="D118"/>
       <c r="E118" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F118" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G118" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="119">
@@ -3481,20 +3017,16 @@
       <c r="B119" t="s">
         <v>131</v>
       </c>
-      <c r="C119" t="n">
-        <v>0</v>
-      </c>
-      <c r="D119" t="n">
-        <v>3</v>
-      </c>
+      <c r="C119"/>
+      <c r="D119"/>
       <c r="E119" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F119" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G119" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120">
@@ -3504,20 +3036,16 @@
       <c r="B120" t="s">
         <v>132</v>
       </c>
-      <c r="C120" t="n">
-        <v>2</v>
-      </c>
-      <c r="D120" t="n">
-        <v>0</v>
-      </c>
+      <c r="C120"/>
+      <c r="D120"/>
       <c r="E120" t="n">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="F120" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G120" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="121">
@@ -3527,14 +3055,10 @@
       <c r="B121" t="s">
         <v>133</v>
       </c>
-      <c r="C121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D121" t="n">
-        <v>1</v>
-      </c>
+      <c r="C121"/>
+      <c r="D121"/>
       <c r="E121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F121" t="s">
         <v>9</v>
@@ -3550,12 +3074,8 @@
       <c r="B122" t="s">
         <v>134</v>
       </c>
-      <c r="C122" t="n">
-        <v>1</v>
-      </c>
-      <c r="D122" t="n">
-        <v>0</v>
-      </c>
+      <c r="C122"/>
+      <c r="D122"/>
       <c r="E122" t="n">
         <v>1</v>
       </c>
@@ -3573,20 +3093,16 @@
       <c r="B123" t="s">
         <v>135</v>
       </c>
-      <c r="C123" t="n">
-        <v>23</v>
-      </c>
-      <c r="D123" t="n">
-        <v>78</v>
-      </c>
+      <c r="C123"/>
+      <c r="D123"/>
       <c r="E123" t="n">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="F123" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G123" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="124">
@@ -3596,20 +3112,16 @@
       <c r="B124" t="s">
         <v>136</v>
       </c>
-      <c r="C124" t="n">
-        <v>3</v>
-      </c>
-      <c r="D124" t="n">
-        <v>3</v>
-      </c>
+      <c r="C124"/>
+      <c r="D124"/>
       <c r="E124" t="n">
         <v>6</v>
       </c>
       <c r="F124" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G124" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="125">
@@ -3619,20 +3131,16 @@
       <c r="B125" t="s">
         <v>137</v>
       </c>
-      <c r="C125" t="n">
-        <v>33</v>
-      </c>
-      <c r="D125" t="n">
-        <v>17</v>
-      </c>
+      <c r="C125"/>
+      <c r="D125"/>
       <c r="E125" t="n">
         <v>50</v>
       </c>
       <c r="F125" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G125" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="126">
@@ -3642,12 +3150,8 @@
       <c r="B126" t="s">
         <v>138</v>
       </c>
-      <c r="C126" t="n">
-        <v>129</v>
-      </c>
-      <c r="D126" t="n">
-        <v>353</v>
-      </c>
+      <c r="C126"/>
+      <c r="D126"/>
       <c r="E126" t="n">
         <v>482</v>
       </c>
@@ -3657,6 +3161,74 @@
       <c r="G126" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="127">
+      <c r="A127"/>
+      <c r="B127" t="s">
+        <v>8</v>
+      </c>
+      <c r="C127" t="n">
+        <v>1</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" t="n">
+        <v>1</v>
+      </c>
+      <c r="F127"/>
+      <c r="G127"/>
+    </row>
+    <row r="128">
+      <c r="A128"/>
+      <c r="B128" t="s">
+        <v>117</v>
+      </c>
+      <c r="C128" t="n">
+        <v>0</v>
+      </c>
+      <c r="D128" t="n">
+        <v>1</v>
+      </c>
+      <c r="E128" t="n">
+        <v>1</v>
+      </c>
+      <c r="F128"/>
+      <c r="G128"/>
+    </row>
+    <row r="129">
+      <c r="A129"/>
+      <c r="B129" t="s">
+        <v>10</v>
+      </c>
+      <c r="C129" t="n">
+        <v>1</v>
+      </c>
+      <c r="D129" t="n">
+        <v>0</v>
+      </c>
+      <c r="E129" t="n">
+        <v>1</v>
+      </c>
+      <c r="F129"/>
+      <c r="G129"/>
+    </row>
+    <row r="130">
+      <c r="A130"/>
+      <c r="B130" t="s">
+        <v>11</v>
+      </c>
+      <c r="C130" t="n">
+        <v>0</v>
+      </c>
+      <c r="D130" t="n">
+        <v>2</v>
+      </c>
+      <c r="E130" t="n">
+        <v>2</v>
+      </c>
+      <c r="F130"/>
+      <c r="G130"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>